<commit_message>
adding improvements in document
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
   <si>
     <t>do not print this form</t>
   </si>
@@ -211,6 +211,61 @@
     <t>After/Argument</t>
   </si>
   <si>
+    <t>ArrayTaskList.java, line 141</t>
+  </si>
+  <si>
+    <t>variable Task overrides the class private variable</t>
+  </si>
+  <si>
+    <t>ArrayTaskList tasks = new ArrayTaskList();</t>
+  </si>
+  <si>
+    <t>ArrayTaskList newTasks = new ArrayTaskList();</t>
+  </si>
+  <si>
+    <t>TaskList.java, line 15</t>
+  </si>
+  <si>
+    <t>"iterator" is defined in the "Iterable" interface</t>
+  </si>
+  <si>
+    <t>public abstract Iterator&lt;Task&gt; iterator();</t>
+  </si>
+  <si>
+    <t>removed</t>
+  </si>
+  <si>
+    <t>TaskIO.java, line 275</t>
+  </si>
+  <si>
+    <t>declare "j" on a seperate line</t>
+  </si>
+  <si>
+    <t>int i = 0, j = time.length-1;</t>
+  </si>
+  <si>
+    <t>int i = 0;
+int j = time.length-1;</t>
+  </si>
+  <si>
+    <t>TaskService.java, line 50</t>
+  </si>
+  <si>
+    <t>block of comment inside method</t>
+  </si>
+  <si>
+    <t>//Iterable&lt;Task&gt; filtered = tasks.incoming(start, end);</t>
+  </si>
+  <si>
+    <t>Main.java, line 28</t>
+  </si>
+  <si>
+    <t>unusued "classLoader"</t>
+  </si>
+  <si>
+    <t>private static ClassLoader classLoader = Main.class.getClassLoader();</t>
+  </si>
+  <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
   </si>
 </sst>
@@ -344,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -406,6 +461,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -22732,8 +22790,12 @@
       <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="I3" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="30">
+        <v>235.0</v>
+      </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
@@ -22764,8 +22826,12 @@
       <c r="H4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="I4" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="30">
+        <v>235.0</v>
+      </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
@@ -22944,10 +23010,18 @@
       <c r="B10" s="8">
         <v>1.0</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="C10" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -22975,10 +23049,18 @@
         <f t="shared" ref="B11:B30" si="1">B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="C11" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -23006,10 +23088,18 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
+      <c r="C12" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>76</v>
+      </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -23037,10 +23127,18 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="C13" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -23068,10 +23166,18 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="C14" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -23620,10 +23726,10 @@
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="30" t="s">
-        <v>65</v>
+      <c r="C32" s="31" t="s">
+        <v>83</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>

</xml_diff>